<commit_message>
Third day's commit_Till data table
</commit_message>
<xml_diff>
--- a/Neha_Pant.xlsx
+++ b/Neha_Pant.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="7752" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="day 1" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="106">
   <si>
     <t>S.No</t>
   </si>
@@ -273,6 +273,76 @@
   </si>
   <si>
     <t>Documentation</t>
+  </si>
+  <si>
+    <t>1st Mar,2017</t>
+  </si>
+  <si>
+    <t>Self Study for DAO</t>
+  </si>
+  <si>
+    <t>Mock</t>
+  </si>
+  <si>
+    <t>Understanding OOD</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=9fVQ_mvzV48  https://www.youtube.com/watch?v=H1mePFyqqiE</t>
+  </si>
+  <si>
+    <t>https://www.codeproject.com/Articles/93369/How-I-explained-OOD-to-my-wife</t>
+  </si>
+  <si>
+    <t>Creating IProductDAO and ProductDAOImpl</t>
+  </si>
+  <si>
+    <t>Creating Model class for Product</t>
+  </si>
+  <si>
+    <t>Creating Model class for Category</t>
+  </si>
+  <si>
+    <t>Creating ICategoryDAO and CategoryDAOImpl</t>
+  </si>
+  <si>
+    <t>Linking DAO with controller</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=STi8nP7yArs</t>
+  </si>
+  <si>
+    <t>Core_Tag_Error</t>
+  </si>
+  <si>
+    <t>JSTL for core tags not found</t>
+  </si>
+  <si>
+    <t>add dependency in pom.xml :   &lt;dependency&gt;
+    &lt;groupId&gt;jstl&lt;/groupId&gt;
+    &lt;artifactId&gt;jstl&lt;/artifactId&gt;
+    &lt;version&gt;1.2&lt;/version&gt;
+    &lt;/dependency&gt;</t>
+  </si>
+  <si>
+    <t>List as datasource for table in products.jsp</t>
+  </si>
+  <si>
+    <t>Route to ProductDetails page from Products page</t>
+  </si>
+  <si>
+    <t>Image_Visibility_Error</t>
+  </si>
+  <si>
+    <t>Core_Tag_Error,Image_Visibility_Error</t>
+  </si>
+  <si>
+    <t>We only specified names of images in list,whicle fetching we used static resources references to access them ,eg: ${images}/${product.productImage}</t>
+  </si>
+  <si>
+    <t>Image non visible in jsp</t>
+  </si>
+  <si>
+    <t>Session on bower,node,data table</t>
   </si>
 </sst>
 </file>
@@ -386,7 +456,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -433,6 +503,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -735,7 +808,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -743,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView topLeftCell="D20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="B23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1307,6 +1380,288 @@
         <v>19</v>
       </c>
     </row>
+    <row r="22" spans="1:8" ht="57.6">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="28.8">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="28.8">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="28.8">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="28.8">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="28.8">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="28.8">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="28.8">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="28.8">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="28.8">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="28.8">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="28.8">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1" display="https://www.youtube.com/watch?v=wx1UU7hhvbA"/>
@@ -1317,9 +1672,10 @@
     <hyperlink ref="D17" r:id="rId6"/>
     <hyperlink ref="D18" r:id="rId7"/>
     <hyperlink ref="D20" r:id="rId8"/>
+    <hyperlink ref="D22" r:id="rId9" display="https://www.youtube.com/watch?v=9fVQ_mvzV48 "/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -1328,7 +1684,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1382,17 +1738,33 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="63" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+    <row r="4" spans="1:4" ht="71.400000000000006" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="63" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="63" customHeight="1">
       <c r="A6" s="3"/>
@@ -1418,7 +1790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="A1:D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
2nd march 2017 commit
</commit_message>
<xml_diff>
--- a/Neha_Pant.xlsx
+++ b/Neha_Pant.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="119">
   <si>
     <t>S.No</t>
   </si>
@@ -343,6 +343,45 @@
   </si>
   <si>
     <t>Session on bower,node,data table</t>
+  </si>
+  <si>
+    <t>ContextComponentScan_Error</t>
+  </si>
+  <si>
+    <t>Multiple annotations found at this line: - schema_reference.4: Failed to read schema document 'http://www.springframework.org/schema/context/spring-context-3.0.xsd', because 1)   could not find the document; 2) the document could not be read; 3) the root element of the document is not &lt;xsd:schema&gt;. - cvc-complex-type.2.4.c: The matching wildcard is strict, but no declaration can be found for element 'context:component-scan'.</t>
+  </si>
+  <si>
+    <t>http://stackoverflow.com/questions/28895990/schema-reference-failed-to-read-schema</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>2nd Mar,2017</t>
+  </si>
+  <si>
+    <t>adding spring dependency for using hibernate with H2</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/org.springframework/spring-orm/4.2.2.RELEASE https://commons.apache.org/proper/commons-dbcp/ https://mvnrepository.com/artifact/org.springframework/spring-orm/5.0.0.M5</t>
+  </si>
+  <si>
+    <t>240 minutes</t>
+  </si>
+  <si>
+    <t>adding applicationContext.xml and connect it using web.xml</t>
+  </si>
+  <si>
+    <t>Put some sample data in the table and it should be retrieved in the Products Page in the datatable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Beans for DataSource, SessionFactory, TransactionManager in applicationContext.xml file. </t>
+  </si>
+  <si>
+    <t>Write the Junit test cases for checking the DAO classes</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
@@ -456,7 +495,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -504,6 +543,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -808,7 +850,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -816,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1650,8 +1692,23 @@
       <c r="C32" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="28.8">
+      <c r="D32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="28.8">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1660,6 +1717,139 @@
       </c>
       <c r="C33" s="1" t="s">
         <v>105</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="57.6">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="28.8">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="57.6">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="43.2">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="28.8">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1683,8 +1873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A4" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1767,10 +1957,18 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="63" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" s="1"/>

</xml_diff>